<commit_message>
Partial fix for date handling
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1_with_date.xlsx
+++ b/storage/test_data/etl/d1_with_date.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">S:date completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:calculated</t>
   </si>
   <si>
     <t xml:space="preserve">DOUBLES1</t>
@@ -52,7 +55,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY\ HH:MM\ AM/PM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -155,7 +158,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -191,7 +194,9 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0"/>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
@@ -215,7 +220,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -227,7 +232,11 @@
         <v>43894</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">C2+D2</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add check for number of blank rows and a check for blank entities so that we can determine when to exit processing loop.
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1_with_date.xlsx
+++ b/storage/test_data/etl/d1_with_date.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -44,18 +44,16 @@
   </si>
   <si>
     <t xml:space="preserve">DOUBLES1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 03/05/20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY\ HH:MM\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -123,7 +121,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,6 +131,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,17 +160,17 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="0" width="8.84"/>
@@ -231,8 +233,8 @@
       <c r="E2" s="2" t="n">
         <v>43894</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>8</v>
+      <c r="F2" s="3" t="n">
+        <v>43895</v>
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">C2+D2</f>

</xml_diff>